<commit_message>
Review màn hình đơn yêu cầu đổi trả, danh sách đơn yêu cầu đổi trả và chi tiết đơn yêu cầu đổi trả
</commit_message>
<xml_diff>
--- a/BaoCao_Review/Interface/[Team1][RV_GUI]QuanLiNPP_DoiTraHangHoa.xlsx
+++ b/BaoCao_Review/Interface/[Team1][RV_GUI]QuanLiNPP_DoiTraHangHoa.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nam4-hk1\hiendai\TH2014-1-PTUDHTTTHD-SaveMyLife-SML\BaoCao_Review\Interface\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\homework\PTHTTTHD\project\TH2014-1-PTUDHTTTHD-SaveMyLife-SML\BaoCao_Review\Interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" tabRatio="475"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" tabRatio="475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inspection" sheetId="9" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Template Revision history'!$A$1:$F$26</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Walk-through'!$A$1:$Y$127</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="327">
   <si>
     <t>Inform to:</t>
   </si>
@@ -1656,11 +1656,40 @@
   <si>
     <t>[Team1][Interface]QuanLiNPP_QuanLiDoiTra</t>
   </si>
+  <si>
+    <t>Nguyễn Thị Thanh Thảo</t>
+  </si>
+  <si>
+    <t>Thêm mã sản phẩm vào danh sách sản phẩm đổi trả
+Thêm khung tìm kiếm sản phẩm để người dùng chọn thay vì nhập tay. Tham khảo màn hình lập đơn đặt hàng</t>
+  </si>
+  <si>
+    <t>Màn hình lập đơn yêu cầu đổi trả</t>
+  </si>
+  <si>
+    <t>Màn hình Chi tiết đơn đổi trả và Chi tiết phiếu đổi trả</t>
+  </si>
+  <si>
+    <t>Thiếu mã sản phẩm trong danh sách sản phẩm đổi trả
+Thiếu tổng tiền
+Người dùng k thể nhớ tên, mã sản phẩm hết đc
+nên không cho nhập tay mà làm thêm 1 khung tìm kiếm sản phẩm cho người dùng chọn.  Tham khảo màn hình lập đơn đặt hàng.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiếu mã sản phẩm trong danh sách sản phẩm đổi trả
+Thiếu tổng tiền ở màn hình Chi tiết đơn đổi trả
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thêm mã sản phẩm vào danh sách sản phẩm đổi trả ở cả 2 màn hình
+Thêm tổng tiền vào Chi tiết đơn đổi trả
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="10">
     <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="165" formatCode="0.00_ "/>
@@ -4348,16 +4377,16 @@
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 2" xfId="1"/>
-    <cellStyle name="標準 3" xfId="9"/>
-    <cellStyle name="標準 4" xfId="10"/>
-    <cellStyle name="標準_コードレビューに関するコメント_コードレビューチェックリストv0.22" xfId="2"/>
-    <cellStyle name="標準_レビューチェックリスト_CD" xfId="3"/>
-    <cellStyle name="標準_レビューチェックリスト_テスト仕様書" xfId="5"/>
-    <cellStyle name="標準_レビューチェックリスト_テスト前" xfId="6"/>
-    <cellStyle name="標準_レビューチェックリスト_テスト結果" xfId="4"/>
-    <cellStyle name="標準_レビューチェックリスト_機能仕様書" xfId="7"/>
-    <cellStyle name="標準_レビューチェックリスト_設計書" xfId="8"/>
+    <cellStyle name="標準 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="標準 3" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="標準 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="標準_コードレビューに関するコメント_コードレビューチェックリストv0.22" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="標準_レビューチェックリスト_CD" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="標準_レビューチェックリスト_テスト仕様書" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="標準_レビューチェックリスト_テスト前" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="標準_レビューチェックリスト_テスト結果" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="標準_レビューチェックリスト_機能仕様書" xfId="7" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="標準_レビューチェックリスト_設計書" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="98">
     <dxf>
@@ -5009,7 +5038,7 @@
         <xdr:cNvPr id="6145" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001180000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001180000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5077,7 +5106,7 @@
         <xdr:cNvPr id="6146" name="正方形/長方形 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002180000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002180000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6284,7 +6313,7 @@
         <xdr:cNvPr id="6147" name="正方形/長方形 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003180000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003180000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6459,7 +6488,7 @@
         <xdr:cNvPr id="10" name="正方形/長方形 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8108,7 +8137,7 @@
         <xdr:cNvPr id="11" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11485,7 +11514,7 @@
         <xdr:cNvPr id="15" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EF028B0C-D360-49E4-8A51-5DDD9991BE88}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF028B0C-D360-49E4-8A51-5DDD9991BE88}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11887,7 +11916,7 @@
         <xdr:cNvPr id="7169" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-0000011C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000011C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11955,7 +11984,7 @@
         <xdr:cNvPr id="7170" name="正方形/長方形 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-0000021C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000021C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12918,7 +12947,7 @@
         <xdr:cNvPr id="10" name="正方形/長方形 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13093,7 +13122,7 @@
         <xdr:cNvPr id="11" name="正方形/長方形 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14749,7 +14778,7 @@
         <xdr:cNvPr id="8" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16883,7 +16912,7 @@
         <xdr:cNvPr id="9" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1D8941C5-C0B8-4AFE-9187-051FAF622739}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D8941C5-C0B8-4AFE-9187-051FAF622739}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17285,7 +17314,7 @@
         <xdr:cNvPr id="2" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79A14699-8D8D-4528-A314-7338B8F61820}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79A14699-8D8D-4528-A314-7338B8F61820}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17349,22 +17378,6 @@
             </a:rPr>
             <a:t>■Additional description</a:t>
           </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:uLnTx/>
-              <a:uFillTx/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
           <a:br>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
               <a:ln>
@@ -18136,7 +18149,7 @@
         <xdr:cNvPr id="3" name="正方形/長方形 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1A8EF14B-5FF3-47E1-8D9B-66E826AF88DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A8EF14B-5FF3-47E1-8D9B-66E826AF88DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18334,15 +18347,6 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>", or "N/A.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="ＭＳ Ｐゴシック" panose="020B0600070205080204" pitchFamily="50" charset="-128"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t/>
           </a:r>
           <a:br>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" baseline="0">
@@ -18721,6 +18725,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -18756,6 +18777,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -18931,15 +18969,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AN81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29:V29"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q36" sqref="Q36:V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -20069,16 +20107,22 @@
       <c r="X33" s="273"/>
       <c r="Y33" s="274"/>
     </row>
-    <row r="34" spans="1:26" ht="42" customHeight="1">
+    <row r="34" spans="1:26" ht="95.25" customHeight="1">
       <c r="B34" s="241">
         <v>7</v>
       </c>
       <c r="C34" s="242" t="s">
         <v>26</v>
       </c>
-      <c r="D34" s="243"/>
-      <c r="E34" s="244"/>
-      <c r="F34" s="269"/>
+      <c r="D34" s="243" t="s">
+        <v>322</v>
+      </c>
+      <c r="E34" s="244" t="s">
+        <v>320</v>
+      </c>
+      <c r="F34" s="269" t="s">
+        <v>324</v>
+      </c>
       <c r="G34" s="270"/>
       <c r="H34" s="270"/>
       <c r="I34" s="270"/>
@@ -20093,7 +20137,9 @@
       <c r="N34" s="239"/>
       <c r="O34" s="271"/>
       <c r="P34" s="272"/>
-      <c r="Q34" s="275"/>
+      <c r="Q34" s="275" t="s">
+        <v>321</v>
+      </c>
       <c r="R34" s="276"/>
       <c r="S34" s="276"/>
       <c r="T34" s="276"/>
@@ -20110,9 +20156,15 @@
       <c r="C35" s="242" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="243"/>
-      <c r="E35" s="244"/>
-      <c r="F35" s="269"/>
+      <c r="D35" s="243" t="s">
+        <v>323</v>
+      </c>
+      <c r="E35" s="244" t="s">
+        <v>320</v>
+      </c>
+      <c r="F35" s="269" t="s">
+        <v>325</v>
+      </c>
       <c r="G35" s="270"/>
       <c r="H35" s="270"/>
       <c r="I35" s="270"/>
@@ -20127,7 +20179,9 @@
       <c r="N35" s="239"/>
       <c r="O35" s="271"/>
       <c r="P35" s="272"/>
-      <c r="Q35" s="275"/>
+      <c r="Q35" s="275" t="s">
+        <v>326</v>
+      </c>
       <c r="R35" s="276"/>
       <c r="S35" s="276"/>
       <c r="T35" s="276"/>
@@ -21754,19 +21808,19 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN76">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN76" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"(Select from list),$J$120,$J$121,$J$122,$J$123,$J$125"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X17:Y25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X17:Y25" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"(Select from list),Line,Page,Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M28:M75">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M28:M75" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"(Select from list),Defect,Risk,Problem,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28:C75">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28:C75" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"(Select from list),①,②,③,④,⑤,⑥,⑦,⑧,⑨,⑩"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L28:L75">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L28:L75" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"(Select from list),Issue,Question"</formula1>
     </dataValidation>
   </dataValidations>
@@ -21780,7 +21834,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
     <pageSetUpPr fitToPage="1"/>
@@ -26465,25 +26519,25 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:M17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:M17" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"(Select from list),Yes (Attached to this template), Yes (project)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X24:Y33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X24:Y33" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"(Select from list),Line,Page,Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M39:M88">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M39:M88" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"(Select from list),Defect,Risk,Problem,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C39:C88">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C39:C88" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"(Select from list),①,②,③,④,⑤,⑥,⑦,⑧,⑨,⑩"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L39:L88">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L39:L88" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"(Select from list),Issue,Question"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J113:Y113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J113:Y113" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>"(Select from list),A,B,C,D,E,F"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T106:Y107">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T106:Y107" xr:uid="{00000000-0002-0000-0100-000006000000}">
       <formula1>" (Select from list),A,B"</formula1>
     </dataValidation>
   </dataValidations>
@@ -26520,7 +26574,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
     <pageSetUpPr fitToPage="1"/>
@@ -30968,25 +31022,25 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:M17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:M17" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"(Select from list),Yes (Attached to this template), Yes (project)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X24:Y33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X24:Y33" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"(Select from list),Line,Page,Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M39:M88">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M39:M88" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"(Select from list),Defect,Risk,Problem,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C39:C88">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C39:C88" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"(Select from list),①,②,③,④,⑤,⑥,⑦,⑧,⑨,⑩"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L39:L88">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L39:L88" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>"(Select from list),Issue,Question"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J112:Y112">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J112:Y112" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>"(Select from list),A,B,C,D,E,F"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T106:Y106">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T106:Y106" xr:uid="{00000000-0002-0000-0200-000006000000}">
       <formula1>" (Select from list),A,B"</formula1>
     </dataValidation>
   </dataValidations>
@@ -31004,7 +31058,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:H171"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
@@ -33703,7 +33757,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E10 E15:E20 E155:E158 E91:E96 E123 E146:E150 E163:E170 E42:E52 E27 E25 E34:E37 E39:E40 E29:E31 E57 E59 E61:E63 E139 E71:E72 E74:E83 E85:E89 E102:E112 E114 E116:E118 E120:E121 E128:E129 E141:E144 E133:E135 E131 E137 E65:E69">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E10 E15:E20 E155:E158 E91:E96 E123 E146:E150 E163:E170 E42:E52 E27 E25 E34:E37 E39:E40 E29:E31 E57 E59 E61:E63 E139 E71:E72 E74:E83 E85:E89 E102:E112 E114 E116:E118 E120:E121 E128:E129 E141:E144 E133:E135 E131 E137 E65:E69" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"(Select from list),○,×,N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -33727,7 +33781,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Review giao diện phiếu đổi trả, phiếu công nợ, phiếu chi
</commit_message>
<xml_diff>
--- a/BaoCao_Review/Interface/[Team1][RV_GUI]QuanLiNPP_DoiTraHangHoa.xlsx
+++ b/BaoCao_Review/Interface/[Team1][RV_GUI]QuanLiNPP_DoiTraHangHoa.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester 7\PTUD HTTT\Project\TH2014-1-PTUDHTTTHD-SaveMyLife-SML\BaoCao_Review\Interface\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Học tập\Học kỳ 7\PT Ứng dụng HTTT hiện đại\Đồ án\TH2014-1-PTUDHTTTHD-SaveMyLife-SML\BaoCao_Review\Interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,12 +25,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Template Revision history'!$A$1:$F$26</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Walk-through'!$A$1:$Y$127</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="336">
   <si>
     <t>Inform to:</t>
   </si>
@@ -1582,9 +1582,6 @@
     <t>Thiết kế</t>
   </si>
   <si>
-    <t>thiết kế chi tiết chức năng hệ thống ( Phần giao diện)</t>
-  </si>
-  <si>
     <t>Các màn hình tìm kiếm</t>
   </si>
   <si>
@@ -1688,11 +1685,42 @@
   <si>
     <t>Nguyễn Hà Tiên</t>
   </si>
+  <si>
+    <t>Màn hình chi tiết phiếu đổi trả</t>
+  </si>
+  <si>
+    <t>Trần Thùy Bích Trâm</t>
+  </si>
+  <si>
+    <t>Võ Thị Thanh Trúc</t>
+  </si>
+  <si>
+    <t>Màn hình phiếu công nợ</t>
+  </si>
+  <si>
+    <t>Thiếu mã sản phẩm trong danh sách sản phẩm đổi trả
+Nên để mã đơn yêu cầu đổi trả lên trên thông tin của nhà phân phối</t>
+  </si>
+  <si>
+    <t>Thêm mã sản phẩm vào danh sách sản phẩm đổi trả
+Để mã đơn yêu cầu đổi trả lên trên thông tin nhà phân phối</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiếu mã phiếu công nợ
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thêm mã phiếu công nợ
+</t>
+  </si>
+  <si>
+    <t>Thiết kế chi tiết chức năng hệ thống ( Phần giao diện)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="10">
     <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="165" formatCode="0.00_ "/>
@@ -5041,7 +5069,7 @@
         <xdr:cNvPr id="6145" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001180000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001180000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5109,7 +5137,7 @@
         <xdr:cNvPr id="6146" name="正方形/長方形 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002180000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002180000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6316,7 +6344,7 @@
         <xdr:cNvPr id="6147" name="正方形/長方形 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003180000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003180000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6491,7 +6519,7 @@
         <xdr:cNvPr id="10" name="正方形/長方形 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8140,7 +8168,7 @@
         <xdr:cNvPr id="11" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11517,7 +11545,7 @@
         <xdr:cNvPr id="15" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF028B0C-D360-49E4-8A51-5DDD9991BE88}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF028B0C-D360-49E4-8A51-5DDD9991BE88}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11919,7 +11947,7 @@
         <xdr:cNvPr id="7169" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000011C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000011C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11987,7 +12015,7 @@
         <xdr:cNvPr id="7170" name="正方形/長方形 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000021C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000021C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12950,7 +12978,7 @@
         <xdr:cNvPr id="10" name="正方形/長方形 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13125,7 +13153,7 @@
         <xdr:cNvPr id="11" name="正方形/長方形 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14781,7 +14809,7 @@
         <xdr:cNvPr id="8" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16915,7 +16943,7 @@
         <xdr:cNvPr id="9" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D8941C5-C0B8-4AFE-9187-051FAF622739}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D8941C5-C0B8-4AFE-9187-051FAF622739}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17317,7 +17345,7 @@
         <xdr:cNvPr id="2" name="正方形/長方形 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79A14699-8D8D-4528-A314-7338B8F61820}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79A14699-8D8D-4528-A314-7338B8F61820}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17381,6 +17409,22 @@
             </a:rPr>
             <a:t>■Additional description</a:t>
           </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
               <a:ln>
@@ -18152,7 +18196,7 @@
         <xdr:cNvPr id="3" name="正方形/長方形 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A8EF14B-5FF3-47E1-8D9B-66E826AF88DF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A8EF14B-5FF3-47E1-8D9B-66E826AF88DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18350,6 +18394,15 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>", or "N/A.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="ＭＳ Ｐゴシック" panose="020B0600070205080204" pitchFamily="50" charset="-128"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t/>
           </a:r>
           <a:br>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" baseline="0">
@@ -18728,23 +18781,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -18780,23 +18816,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -18979,8 +18998,8 @@
   </sheetPr>
   <dimension ref="A1:AN81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A32" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28:P33"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17:W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -19030,7 +19049,7 @@
       <c r="R1" s="288"/>
       <c r="S1" s="289"/>
       <c r="T1" s="287" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="U1" s="288"/>
       <c r="V1" s="288"/>
@@ -19245,12 +19264,12 @@
       <c r="R8" s="216"/>
       <c r="S8" s="217"/>
       <c r="T8" s="315" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="U8" s="316"/>
       <c r="V8" s="317"/>
       <c r="W8" s="315" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="X8" s="316"/>
       <c r="Y8" s="317"/>
@@ -19448,7 +19467,7 @@
       </c>
       <c r="G16" s="339"/>
       <c r="H16" s="328" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I16" s="328"/>
       <c r="J16" s="339" t="s">
@@ -19456,7 +19475,7 @@
       </c>
       <c r="K16" s="339"/>
       <c r="L16" s="328" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M16" s="328"/>
       <c r="N16" s="339" t="s">
@@ -19489,7 +19508,7 @@
       </c>
       <c r="G17" s="339"/>
       <c r="H17" s="327" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I17" s="328"/>
       <c r="J17" s="328"/>
@@ -19504,7 +19523,7 @@
       <c r="S17" s="281"/>
       <c r="T17" s="281"/>
       <c r="U17" s="283">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="V17" s="283"/>
       <c r="W17" s="283"/>
@@ -19573,7 +19592,7 @@
       </c>
       <c r="K19" s="347"/>
       <c r="L19" s="344" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M19" s="344"/>
       <c r="N19" s="282" t="s">
@@ -19581,7 +19600,7 @@
       </c>
       <c r="O19" s="282"/>
       <c r="P19" s="345" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q19" s="346"/>
       <c r="R19" s="281"/>
@@ -19635,7 +19654,7 @@
       </c>
       <c r="C21" s="286"/>
       <c r="D21" s="284" t="s">
-        <v>295</v>
+        <v>335</v>
       </c>
       <c r="E21" s="284"/>
       <c r="F21" s="284"/>
@@ -19645,7 +19664,7 @@
       <c r="J21" s="284"/>
       <c r="K21" s="284"/>
       <c r="L21" s="284" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M21" s="284"/>
       <c r="N21" s="284"/>
@@ -19868,13 +19887,13 @@
         <v>26</v>
       </c>
       <c r="D28" s="243" t="s">
+        <v>295</v>
+      </c>
+      <c r="E28" s="244" t="s">
         <v>296</v>
       </c>
-      <c r="E28" s="244" t="s">
+      <c r="F28" s="349" t="s">
         <v>297</v>
-      </c>
-      <c r="F28" s="349" t="s">
-        <v>298</v>
       </c>
       <c r="G28" s="350"/>
       <c r="H28" s="350"/>
@@ -19888,14 +19907,14 @@
         <v>292</v>
       </c>
       <c r="N28" s="239" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O28" s="276">
         <v>43058</v>
       </c>
       <c r="P28" s="277"/>
       <c r="Q28" s="357" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="R28" s="274"/>
       <c r="S28" s="274"/>
@@ -19914,13 +19933,13 @@
         <v>26</v>
       </c>
       <c r="D29" s="243" t="s">
+        <v>299</v>
+      </c>
+      <c r="E29" s="244" t="s">
+        <v>296</v>
+      </c>
+      <c r="F29" s="349" t="s">
         <v>300</v>
-      </c>
-      <c r="E29" s="244" t="s">
-        <v>297</v>
-      </c>
-      <c r="F29" s="349" t="s">
-        <v>301</v>
       </c>
       <c r="G29" s="350"/>
       <c r="H29" s="350"/>
@@ -19934,14 +19953,14 @@
         <v>292</v>
       </c>
       <c r="N29" s="239" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O29" s="276">
         <v>43058</v>
       </c>
       <c r="P29" s="277"/>
       <c r="Q29" s="273" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="R29" s="274"/>
       <c r="S29" s="274"/>
@@ -19960,13 +19979,13 @@
         <v>26</v>
       </c>
       <c r="D30" s="243" t="s">
+        <v>301</v>
+      </c>
+      <c r="E30" s="244" t="s">
+        <v>296</v>
+      </c>
+      <c r="F30" s="349" t="s">
         <v>302</v>
-      </c>
-      <c r="E30" s="244" t="s">
-        <v>297</v>
-      </c>
-      <c r="F30" s="349" t="s">
-        <v>303</v>
       </c>
       <c r="G30" s="350"/>
       <c r="H30" s="350"/>
@@ -19980,14 +19999,14 @@
         <v>292</v>
       </c>
       <c r="N30" s="239" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O30" s="276">
         <v>43058</v>
       </c>
       <c r="P30" s="277"/>
       <c r="Q30" s="273" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="R30" s="274"/>
       <c r="S30" s="274"/>
@@ -20006,13 +20025,13 @@
         <v>26</v>
       </c>
       <c r="D31" s="243" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E31" s="244" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F31" s="349" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G31" s="350"/>
       <c r="H31" s="350"/>
@@ -20026,14 +20045,14 @@
         <v>255</v>
       </c>
       <c r="N31" s="239" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O31" s="276">
         <v>43058</v>
       </c>
       <c r="P31" s="277"/>
       <c r="Q31" s="273" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="R31" s="274"/>
       <c r="S31" s="274"/>
@@ -20052,13 +20071,13 @@
         <v>26</v>
       </c>
       <c r="D32" s="243" t="s">
+        <v>308</v>
+      </c>
+      <c r="E32" s="244" t="s">
+        <v>296</v>
+      </c>
+      <c r="F32" s="349" t="s">
         <v>309</v>
-      </c>
-      <c r="E32" s="244" t="s">
-        <v>297</v>
-      </c>
-      <c r="F32" s="349" t="s">
-        <v>310</v>
       </c>
       <c r="G32" s="350"/>
       <c r="H32" s="350"/>
@@ -20072,14 +20091,14 @@
         <v>292</v>
       </c>
       <c r="N32" s="239" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O32" s="276">
         <v>43058</v>
       </c>
       <c r="P32" s="277"/>
       <c r="Q32" s="273" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="R32" s="274"/>
       <c r="S32" s="274"/>
@@ -20098,13 +20117,13 @@
         <v>26</v>
       </c>
       <c r="D33" s="243" t="s">
+        <v>295</v>
+      </c>
+      <c r="E33" s="244" t="s">
         <v>296</v>
       </c>
-      <c r="E33" s="244" t="s">
-        <v>297</v>
-      </c>
       <c r="F33" s="349" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G33" s="350"/>
       <c r="H33" s="350"/>
@@ -20118,14 +20137,14 @@
         <v>292</v>
       </c>
       <c r="N33" s="239" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O33" s="276">
         <v>43058</v>
       </c>
       <c r="P33" s="277"/>
       <c r="Q33" s="273" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="R33" s="274"/>
       <c r="S33" s="274"/>
@@ -20144,13 +20163,13 @@
         <v>26</v>
       </c>
       <c r="D34" s="243" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E34" s="244" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F34" s="349" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G34" s="350"/>
       <c r="H34" s="350"/>
@@ -20163,11 +20182,13 @@
       <c r="M34" s="246" t="s">
         <v>292</v>
       </c>
-      <c r="N34" s="239"/>
+      <c r="N34" s="239" t="s">
+        <v>329</v>
+      </c>
       <c r="O34" s="276"/>
       <c r="P34" s="277"/>
       <c r="Q34" s="273" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R34" s="274"/>
       <c r="S34" s="274"/>
@@ -20186,13 +20207,13 @@
         <v>26</v>
       </c>
       <c r="D35" s="243" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E35" s="244" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F35" s="349" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G35" s="350"/>
       <c r="H35" s="350"/>
@@ -20205,11 +20226,13 @@
       <c r="M35" s="246" t="s">
         <v>292</v>
       </c>
-      <c r="N35" s="239"/>
+      <c r="N35" s="239" t="s">
+        <v>329</v>
+      </c>
       <c r="O35" s="276"/>
       <c r="P35" s="277"/>
       <c r="Q35" s="273" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="R35" s="274"/>
       <c r="S35" s="274"/>
@@ -20220,17 +20243,23 @@
       <c r="X35" s="271"/>
       <c r="Y35" s="272"/>
     </row>
-    <row r="36" spans="1:26" ht="42" customHeight="1">
+    <row r="36" spans="1:26" ht="54.75" customHeight="1">
       <c r="A36" s="233"/>
       <c r="B36" s="241">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" s="242" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="243"/>
-      <c r="E36" s="244"/>
-      <c r="F36" s="349"/>
+      <c r="D36" s="243" t="s">
+        <v>327</v>
+      </c>
+      <c r="E36" s="244" t="s">
+        <v>328</v>
+      </c>
+      <c r="F36" s="349" t="s">
+        <v>331</v>
+      </c>
       <c r="G36" s="350"/>
       <c r="H36" s="350"/>
       <c r="I36" s="350"/>
@@ -20242,10 +20271,14 @@
       <c r="M36" s="246" t="s">
         <v>255</v>
       </c>
-      <c r="N36" s="239"/>
+      <c r="N36" s="239" t="s">
+        <v>329</v>
+      </c>
       <c r="O36" s="276"/>
       <c r="P36" s="277"/>
-      <c r="Q36" s="273"/>
+      <c r="Q36" s="273" t="s">
+        <v>332</v>
+      </c>
       <c r="R36" s="274"/>
       <c r="S36" s="274"/>
       <c r="T36" s="274"/>
@@ -20259,14 +20292,20 @@
     <row r="37" spans="1:26" ht="42" customHeight="1">
       <c r="A37" s="233"/>
       <c r="B37" s="241">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C37" s="242" t="s">
         <v>26</v>
       </c>
-      <c r="D37" s="243"/>
-      <c r="E37" s="244"/>
-      <c r="F37" s="349"/>
+      <c r="D37" s="243" t="s">
+        <v>330</v>
+      </c>
+      <c r="E37" s="244" t="s">
+        <v>328</v>
+      </c>
+      <c r="F37" s="349" t="s">
+        <v>333</v>
+      </c>
       <c r="G37" s="350"/>
       <c r="H37" s="350"/>
       <c r="I37" s="350"/>
@@ -20276,12 +20315,16 @@
         <v>254</v>
       </c>
       <c r="M37" s="246" t="s">
-        <v>292</v>
-      </c>
-      <c r="N37" s="239"/>
+        <v>255</v>
+      </c>
+      <c r="N37" s="239" t="s">
+        <v>329</v>
+      </c>
       <c r="O37" s="276"/>
       <c r="P37" s="277"/>
-      <c r="Q37" s="273"/>
+      <c r="Q37" s="273" t="s">
+        <v>334</v>
+      </c>
       <c r="R37" s="274"/>
       <c r="S37" s="274"/>
       <c r="T37" s="274"/>
@@ -20295,7 +20338,7 @@
     <row r="38" spans="1:26" s="251" customFormat="1" ht="42" customHeight="1">
       <c r="A38" s="250"/>
       <c r="B38" s="241">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C38" s="242" t="s">
         <v>26</v>
@@ -20330,7 +20373,7 @@
     <row r="39" spans="1:26" s="251" customFormat="1" ht="42" customHeight="1">
       <c r="A39" s="250"/>
       <c r="B39" s="241">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C39" s="242" t="s">
         <v>26</v>
@@ -20365,7 +20408,7 @@
     <row r="40" spans="1:26" s="251" customFormat="1" ht="42" customHeight="1">
       <c r="A40" s="250"/>
       <c r="B40" s="241">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C40" s="242" t="s">
         <v>26</v>
@@ -20400,7 +20443,7 @@
     <row r="41" spans="1:26" s="251" customFormat="1" ht="42" customHeight="1">
       <c r="A41" s="250"/>
       <c r="B41" s="241">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C41" s="242" t="s">
         <v>26</v>
@@ -20435,7 +20478,7 @@
     <row r="42" spans="1:26" s="251" customFormat="1" ht="42" customHeight="1">
       <c r="A42" s="250"/>
       <c r="B42" s="241">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C42" s="242" t="s">
         <v>26</v>
@@ -26572,7 +26615,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="68" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;C&amp;9&amp;P/&amp;N</oddFooter>
   </headerFooter>

</xml_diff>